<commit_message>
xong tất cả tài liệu cá nhân
</commit_message>
<xml_diff>
--- a/documents/bikedata_mapping.xlsx
+++ b/documents/bikedata_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChuongTrinhDaiHoc\Data Warehouse\tong_hop_tai_lieu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChuongTrinhDaiHoc\Data Warehouse\datawarehouse_staging\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA5FB0D-0005-4883-91DB-75288FB15D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEB37DC-7C71-4C00-8463-26F05D551C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -372,7 +372,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>